<commit_message>
Add updated microstates from SAMPL6
</commit_message>
<xml_diff>
--- a/microstates/SM01_microstate_IDs_with_2D_depiction.xlsx
+++ b/microstates/SM01_microstate_IDs_with_2D_depiction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Microstate List</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>canonical isomeric SMILES</t>
+  </si>
+  <si>
+    <t>canonical SMILES</t>
   </si>
   <si>
     <t>SM01_micro001</t>
@@ -780,14 +783,15 @@
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="55" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1">
+    <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -797,69 +801,96 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" ht="250.0" customHeight="1">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="250.0" customHeight="1">
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" ht="250.0" customHeight="1">
+    <row r="4" spans="1:4" s="3" customFormat="1" ht="250.0" customHeight="1">
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" ht="250.0" customHeight="1">
+    <row r="5" spans="1:4" s="2" customFormat="1" ht="250.0" customHeight="1">
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" ht="250.0" customHeight="1">
+    <row r="6" spans="1:4" s="3" customFormat="1" ht="250.0" customHeight="1">
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" ht="250.0" customHeight="1">
+    <row r="7" spans="1:4" s="2" customFormat="1" ht="250.0" customHeight="1">
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="3" customFormat="1" ht="250.0" customHeight="1">
+    <row r="8" spans="1:4" s="3" customFormat="1" ht="250.0" customHeight="1">
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" ht="250.0" customHeight="1">
+    <row r="9" spans="1:4" s="2" customFormat="1" ht="250.0" customHeight="1">
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="3" customFormat="1" ht="250.0" customHeight="1">
+    <row r="10" spans="1:4" s="3" customFormat="1" ht="250.0" customHeight="1">
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>